<commit_message>
minor amendments of functions - REMINDER: need to work on the optimization
</commit_message>
<xml_diff>
--- a/xlsx/asset_allocation_chiara_28Mar25.xlsx
+++ b/xlsx/asset_allocation_chiara_28Mar25.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935cc860ba0efd68/GitHub/myportfolio/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="695" documentId="13_ncr:1_{B67B8E68-9111-4423-844A-1B534CD4331C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{446B4663-9CFB-4AFE-8E2E-6B3B1EF1F46E}"/>
+  <xr:revisionPtr revIDLastSave="707" documentId="13_ncr:1_{B67B8E68-9111-4423-844A-1B534CD4331C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE7745EF-31F9-45D7-BF1A-A8172ADE4414}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="1800" windowWidth="17280" windowHeight="8910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUOTE" sheetId="5" r:id="rId1"/>
@@ -1904,13 +1904,13 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.15</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.15</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1919,13 +1919,13 @@
                   <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.08</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.05</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.12</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2830,10 +2830,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3167,23 +3163,23 @@
         <v>World Momentum</v>
       </c>
       <c r="B2" s="24">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="C2" s="10" cm="1">
         <f t="array" ref="C2:C9">MMULT(var_cov!B2:I9,B2:B9)</f>
-        <v>1.1982752741628983E-3</v>
+        <v>1.1091833151008498E-3</v>
       </c>
       <c r="D2" s="10">
         <f t="shared" ref="D2:D8" si="0">C2/$B$15</f>
-        <v>4.4306519631303491E-2</v>
+        <v>4.1572546744470071E-2</v>
       </c>
       <c r="E2" s="11">
         <f>D2*B2</f>
-        <v>1.3291955889391046E-2</v>
+        <v>0</v>
       </c>
       <c r="F2" s="12">
         <f t="shared" ref="F2:F9" si="1">$B$15/9</f>
-        <v>3.005013669255653E-3</v>
+        <v>2.9645186599773243E-3</v>
       </c>
       <c r="G2" s="25" cm="1">
         <f t="array" ref="G2:G9">TRANSPOSE(Returns!B78:I78)</f>
@@ -3191,11 +3187,11 @@
       </c>
       <c r="H2" s="13">
         <f>G2*B2</f>
-        <v>3.1075383672472356E-3</v>
+        <v>0</v>
       </c>
       <c r="I2" s="26">
         <f>(E2-F2)^2</f>
-        <v>1.0582118024040408E-4</v>
+        <v>8.7883708853537512E-6</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -3203,33 +3199,33 @@
         <v>World Quality</v>
       </c>
       <c r="B3" s="24">
-        <v>0.15</v>
+        <v>0.4</v>
       </c>
       <c r="C3" s="10">
-        <v>1.1412965417570593E-3</v>
+        <v>1.1532516196706595E-3</v>
       </c>
       <c r="D3" s="10">
         <f t="shared" si="0"/>
-        <v>4.2199717145814754E-2</v>
+        <v>4.3224240947525569E-2</v>
       </c>
       <c r="E3" s="11">
         <f t="shared" ref="E3:E8" si="2">D3*B3</f>
-        <v>6.3299575718722126E-3</v>
+        <v>1.728969637901023E-2</v>
       </c>
       <c r="F3" s="12">
         <f t="shared" si="1"/>
-        <v>3.005013669255653E-3</v>
+        <v>2.9645186599773243E-3</v>
       </c>
       <c r="G3" s="25">
         <v>9.8206931531271933E-3</v>
       </c>
       <c r="H3" s="13">
         <f t="shared" ref="H3:H9" si="3">G3*B3</f>
-        <v>1.4731039729690789E-3</v>
+        <v>3.9282772612508777E-3</v>
       </c>
       <c r="I3" s="27">
         <f t="shared" ref="I3:I9" si="4">(E3-F3)^2</f>
-        <v>1.1055251955547038E-5</v>
+        <v>2.0521071668187682E-4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -3237,33 +3233,33 @@
         <v>World Low Volatility</v>
       </c>
       <c r="B4" s="24">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="C4" s="10">
-        <v>8.1166902597669995E-4</v>
+        <v>8.2554317510977692E-4</v>
       </c>
       <c r="D4" s="10">
         <f t="shared" si="0"/>
-        <v>3.0011659598567993E-2</v>
+        <v>3.0941623237191396E-2</v>
       </c>
       <c r="E4" s="11">
         <f t="shared" si="2"/>
-        <v>4.5017489397851992E-3</v>
+        <v>6.1883246474382795E-3</v>
       </c>
       <c r="F4" s="12">
         <f t="shared" si="1"/>
-        <v>3.005013669255653E-3</v>
+        <v>2.9645186599773243E-3</v>
       </c>
       <c r="G4" s="25">
         <v>6.3270381497137511E-3</v>
       </c>
       <c r="H4" s="13">
         <f t="shared" si="3"/>
-        <v>9.4905572245706257E-4</v>
+        <v>1.2654076299427504E-3</v>
       </c>
       <c r="I4" s="27">
         <f t="shared" si="4"/>
-        <v>2.2402164700471539E-6</v>
+        <v>1.0392925044789105E-5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -3274,11 +3270,11 @@
         <v>0</v>
       </c>
       <c r="C5" s="10">
-        <v>3.2133466031864568E-4</v>
+        <v>3.356517824071173E-4</v>
       </c>
       <c r="D5" s="10">
         <f t="shared" si="0"/>
-        <v>1.1881427200083283E-2</v>
+        <v>1.2580336562956554E-2</v>
       </c>
       <c r="E5" s="11">
         <f t="shared" si="2"/>
@@ -3286,7 +3282,7 @@
       </c>
       <c r="F5" s="12">
         <f t="shared" si="1"/>
-        <v>3.005013669255653E-3</v>
+        <v>2.9645186599773243E-3</v>
       </c>
       <c r="G5" s="25">
         <v>7.9742200778861036E-5</v>
@@ -3297,7 +3293,7 @@
       </c>
       <c r="I5" s="27">
         <f t="shared" si="4"/>
-        <v>9.030107152413324E-6</v>
+        <v>8.7883708853537512E-6</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -3308,19 +3304,19 @@
         <v>0.15</v>
       </c>
       <c r="C6" s="10">
-        <v>2.7742283406979564E-4</v>
+        <v>2.9449810843541508E-4</v>
       </c>
       <c r="D6" s="10">
         <f t="shared" si="0"/>
-        <v>1.0257776747060106E-2</v>
+        <v>1.1037883650437114E-2</v>
       </c>
       <c r="E6" s="11">
         <f t="shared" si="2"/>
-        <v>1.5386665120590158E-3</v>
+        <v>1.655682547565567E-3</v>
       </c>
       <c r="F6" s="12">
         <f t="shared" si="1"/>
-        <v>3.005013669255653E-3</v>
+        <v>2.9645186599773243E-3</v>
       </c>
       <c r="G6" s="25">
         <v>-1.1366047669321446E-3</v>
@@ -3331,7 +3327,7 @@
       </c>
       <c r="I6" s="27">
         <f t="shared" si="4"/>
-        <v>2.1501739854186593E-6</v>
+        <v>1.7130519691531221E-6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -3339,33 +3335,33 @@
         <v>EU Overnight</v>
       </c>
       <c r="B7" s="24">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="C7" s="10">
-        <v>5.9817227636914333E-6</v>
+        <v>5.6577307460696274E-6</v>
       </c>
       <c r="D7" s="10">
         <f t="shared" si="0"/>
-        <v>2.2117565368579936E-4</v>
+        <v>2.1205356473219175E-4</v>
       </c>
       <c r="E7" s="11">
         <f t="shared" si="2"/>
-        <v>1.7694052294863949E-5</v>
+        <v>2.1205356473219176E-5</v>
       </c>
       <c r="F7" s="12">
         <f t="shared" si="1"/>
-        <v>3.005013669255653E-3</v>
+        <v>2.9645186599773243E-3</v>
       </c>
       <c r="G7" s="25">
         <v>7.574626534542976E-4</v>
       </c>
       <c r="H7" s="13">
         <f t="shared" si="3"/>
-        <v>6.059701227634381E-5</v>
+        <v>7.5746265345429768E-5</v>
       </c>
       <c r="I7" s="27">
         <f t="shared" si="4"/>
-        <v>8.9240784938787548E-6</v>
+        <v>8.6630932025842476E-6</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -3373,33 +3369,33 @@
         <v>US Short Treasury</v>
       </c>
       <c r="B8" s="24">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="C8" s="10">
-        <v>4.0114699329792974E-6</v>
+        <v>3.8852422257360638E-6</v>
       </c>
       <c r="D8" s="10">
         <f t="shared" si="0"/>
-        <v>1.4832507618927054E-4</v>
+        <v>1.4562012594673379E-4</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="2"/>
-        <v>7.416253809463527E-6</v>
+        <v>0</v>
       </c>
       <c r="F8" s="12">
         <f t="shared" si="1"/>
-        <v>3.005013669255653E-3</v>
+        <v>2.9645186599773243E-3</v>
       </c>
       <c r="G8" s="25">
         <v>2.0424847296149273E-3</v>
       </c>
       <c r="H8" s="13">
         <f t="shared" si="3"/>
-        <v>1.0212423648074638E-4</v>
+        <v>0</v>
       </c>
       <c r="I8" s="27">
         <f t="shared" si="4"/>
-        <v>8.9855902650896743E-6</v>
+        <v>8.7883708853537512E-6</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3407,33 +3403,33 @@
         <v>ETC GOLD</v>
       </c>
       <c r="B9" s="24">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="C9" s="10">
-        <v>3.0598937923610129E-4</v>
+        <v>2.7138846322343662E-4</v>
       </c>
       <c r="D9" s="10">
         <f>C9/$B$15</f>
-        <v>1.1314031700742291E-2</v>
+        <v>1.0171726728724186E-2</v>
       </c>
       <c r="E9" s="11">
         <f>D9*B9</f>
-        <v>1.3576838040890748E-3</v>
+        <v>1.5257590093086279E-3</v>
       </c>
       <c r="F9" s="12">
         <f t="shared" si="1"/>
-        <v>3.005013669255653E-3</v>
+        <v>2.9645186599773243E-3</v>
       </c>
       <c r="G9" s="25">
         <v>1.317275007488662E-2</v>
       </c>
       <c r="H9" s="13">
         <f t="shared" si="3"/>
-        <v>1.5807300089863943E-3</v>
+        <v>1.9759125112329928E-3</v>
       </c>
       <c r="I9" s="27">
         <f t="shared" si="4"/>
-        <v>2.7136956846697371E-6</v>
+        <v>2.0700293323923094E-6</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3450,22 +3446,22 @@
       </c>
       <c r="E10" s="17">
         <f>SUM(E2:E9)</f>
-        <v>2.7045123023300872E-2</v>
+        <v>2.6680667939795923E-2</v>
       </c>
       <c r="F10" s="18">
         <f>SUM(F2:F9)</f>
-        <v>2.4040109354045221E-2</v>
+        <v>2.3716149279818598E-2</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>10</v>
       </c>
       <c r="H10" s="20">
         <f>SUM(H2:H9)</f>
-        <v>7.1026586053770414E-3</v>
+        <v>7.0748529527322294E-3</v>
       </c>
       <c r="I10" s="28">
         <f>SUM(I2:I9)</f>
-        <v>1.509202942474684E-4</v>
+        <v>2.5441492888685687E-4</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3480,7 +3476,7 @@
       </c>
       <c r="H11" s="45">
         <f>(H10+1)^12-1</f>
-        <v>8.864155848145705E-2</v>
+        <v>8.8280930385893353E-2</v>
       </c>
       <c r="I11" s="46"/>
     </row>
@@ -3496,7 +3492,7 @@
       </c>
       <c r="B14" s="31" cm="1">
         <f t="array" ref="B14">MMULT(MMULT(TRANSPOSE(B2:B9),var_cov!B2:I9),B2:B9)</f>
-        <v>7.3143867934547912E-4</v>
+        <v>7.118580417136538E-4</v>
       </c>
       <c r="C14" s="42"/>
       <c r="G14" s="43"/>
@@ -3507,7 +3503,7 @@
       </c>
       <c r="B15" s="33">
         <f>SQRT(B14)</f>
-        <v>2.7045123023300876E-2</v>
+        <v>2.668066793979592E-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -3516,7 +3512,7 @@
       </c>
       <c r="B16" s="34">
         <f>SUM(H2:H9)</f>
-        <v>7.1026586053770414E-3</v>
+        <v>7.0748529527322294E-3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3525,7 +3521,7 @@
       </c>
       <c r="B17" s="34">
         <f>(B16+1)^12-1</f>
-        <v>8.864155848145705E-2</v>
+        <v>8.8280930385893353E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -3542,7 +3538,7 @@
       </c>
       <c r="B19" s="50">
         <f>(B17-B18)/B15</f>
-        <v>2.2681190404868148</v>
+        <v>2.2855848483064549</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -3551,7 +3547,7 @@
       </c>
       <c r="B20" s="36">
         <f>I10</f>
-        <v>1.509202942474684E-4</v>
+        <v>2.5441492888685687E-4</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">

</xml_diff>